<commit_message>
im a mad man!!
</commit_message>
<xml_diff>
--- a/Danfoss Heating system/bin/Debug/net8.0/Assets/data.xlsx
+++ b/Danfoss Heating system/bin/Debug/net8.0/Assets/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samgl\Documents\GitHub\smesterProjectSW2\Danfoss Heating system\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kubak\OneDrive\Pulpit\Danfoss Heating System\smesterProjectSW2\Danfoss Heating system\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D13A821-4069-4A15-AC01-300E67D9D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C562C8-3E74-4376-9E35-121E908D78D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19275" yWindow="6345" windowWidth="22035" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Winter period</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Production Units</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Max Heat</t>
   </si>
   <si>
@@ -195,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +226,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -250,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -276,6 +281,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,7 +372,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2564,7 +2570,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="658203504"/>
@@ -2623,7 +2629,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="658202064"/>
@@ -2665,7 +2671,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="948367536"/>
@@ -2734,7 +2740,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2771,7 +2777,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2855,7 +2861,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5053,7 +5059,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="658203504"/>
@@ -5112,7 +5118,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="658202064"/>
@@ -5154,7 +5160,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="948367536"/>
@@ -5223,7 +5229,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5260,7 +5266,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6729,17 +6735,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AB171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="120.28515625" bestFit="1" customWidth="1"/>
@@ -6783,12 +6790,14 @@
       <c r="R1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" t="s">
-        <v>35</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="W1" s="10" t="s">
         <v>36</v>
       </c>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
     </row>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
@@ -6824,23 +6833,23 @@
       <c r="R2" t="s">
         <v>33</v>
       </c>
-      <c r="W2" t="s">
+      <c r="W2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="X2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="8" t="s">
         <v>41</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.25">
@@ -6877,20 +6886,20 @@
       <c r="R3" t="s">
         <v>34</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z3" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="Y3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AA3" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="17.25" x14ac:dyDescent="0.3">
@@ -6927,7 +6936,7 @@
         <v>25</v>
       </c>
       <c r="W4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="X4">
         <v>5</v>
@@ -6979,7 +6988,7 @@
         <v>25</v>
       </c>
       <c r="W5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="X5">
         <v>4</v>
@@ -7031,7 +7040,7 @@
         <v>25</v>
       </c>
       <c r="W6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X6">
         <v>3.6</v>
@@ -7083,7 +7092,7 @@
         <v>25</v>
       </c>
       <c r="W7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="X7">
         <v>8</v>
@@ -11761,9 +11770,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="G1:J1"/>
+    <mergeCell ref="W1:AB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>

</xml_diff>